<commit_message>
Eliminar el table formatter y in cluirlo en el exporter
</commit_message>
<xml_diff>
--- a/exports/resultDScc.xlsx
+++ b/exports/resultDScc.xlsx
@@ -8,6 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pagina" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pagina1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="pagina2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +451,16 @@
           <t>URL</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>File size</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>More info</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -466,7 +478,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/5935EPStudies/epsdtl32139.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/5935EPStudies/eps dtl32139.pdf </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">388 kb </t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= 5935EPStudies </t>
         </is>
       </c>
     </row>
@@ -486,7 +508,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-17/dtl17ss224.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-17/dtl17s s224.pdf </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">117 kb </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-17 </t>
         </is>
       </c>
     </row>
@@ -506,7 +538,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-39030/dtl39030ss20.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-39030/dtl 39030ss20.pdf </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">130 kb </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-39030 </t>
         </is>
       </c>
     </row>
@@ -526,7 +568,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-39030/dtl39030ss21.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-39030/dtl 39030ss21.pdf </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">108 kb </t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-39030 </t>
         </is>
       </c>
     </row>
@@ -546,7 +598,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-83503/dtl83503.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-83503/dtl 83503.pdf </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">288 kb </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-83503 </t>
         </is>
       </c>
     </row>
@@ -566,7 +628,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss30not1.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss3 0not1.pdf </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">61 kb </t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-1 </t>
         </is>
       </c>
     </row>
@@ -586,7 +658,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss148not1.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss1 48not1.pdf </t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">60 kb </t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-1 </t>
         </is>
       </c>
     </row>
@@ -606,7 +688,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss781not1.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss7 81not1.pdf </t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">60 kb </t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-1 </t>
         </is>
       </c>
     </row>
@@ -626,7 +718,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss1047not1.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss1 047not1.pdf </t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">61 kb </t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-1 </t>
         </is>
       </c>
     </row>
@@ -646,7 +748,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss1636.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-1/prf1ss1 636.pdf </t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">278 kb </t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-1 </t>
         </is>
       </c>
     </row>
@@ -666,7 +778,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-19500/idprf19500ss426.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-19500/idp rf19500ss426.pdf </t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">549 kb </t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-19500 </t>
         </is>
       </c>
     </row>
@@ -686,7 +808,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-19500/idprf19500ss439.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-19500/idp rf19500ss439.pdf </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">637 kb </t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-19500 </t>
         </is>
       </c>
     </row>
@@ -706,7 +838,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-19500/idprf19500ss782.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-19500/idp rf19500ss782.pdf </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1007 kb </t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-19500 </t>
         </is>
       </c>
     </row>
@@ -726,7 +868,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-39016/prf39016ss48.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-39016/prf 39016ss48.pdf </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">160 kb </t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-39016 </t>
         </is>
       </c>
     </row>
@@ -746,7 +898,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss39.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf 55339ss39.pdf </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">244 kb </t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-55339 </t>
         </is>
       </c>
     </row>
@@ -766,7 +928,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss48.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf 55339ss48.pdf </t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">116 kb </t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-55339 </t>
         </is>
       </c>
     </row>
@@ -786,7 +958,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss51.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf 55339ss51.pdf </t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">196 kb </t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-55339 </t>
         </is>
       </c>
     </row>
@@ -806,7 +988,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss54.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf 55339ss54.pdf </t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">121 kb </t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-55339 </t>
         </is>
       </c>
     </row>
@@ -826,7 +1018,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf55339ss55.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-55339/prf 55339ss55.pdf </t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">137 kb </t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-55339 </t>
         </is>
       </c>
     </row>
@@ -846,7 +1048,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-6106/idprf6106.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-6106/idpr f6106.pdf </t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">862 kb </t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-6106 </t>
         </is>
       </c>
     </row>
@@ -866,7 +1078,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-6106/idprf6106sup1.pdf</t>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-6106/idpr f6106sup1.pdf </t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">192 kb </t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-6106 </t>
         </is>
       </c>
     </row>
@@ -886,9 +1108,402 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-6106/ms27706.pdf</t>
-        </is>
-      </c>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-PRF-6106/ms27 706.pdf </t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">381 kb </t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-PRF-6106 </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Document</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>File size</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>More info</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EP Study MIL-DTL-32139/15 and /16 -- Dated 4/5/2023 </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Connectors, Electrical, Rectangular, Nanominiature, Dual Row, Plug, Receptacle, Polarized Shell, Pin, Sockets Contacts, Vertical PCB Surface Mount Shell </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/5935EPStudies/eps dtl32139.pdf </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">388 kb </t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= 5935EPStudies </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-DTL-17/224A w/Amendment 1 -- Dated 2/27/2023 </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cable, Radio Frequency, Flexible, Coaxial, 50 Ohms, Low Smoke, Low Loss Diameter .500 </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-17/dtl17s s224.pdf </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">117 kb </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-17 </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-DTL-39030/20D w/Amendment 1 -- Dated 1/31/2023 </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dummy Loads, Electrical Type XIV (Tab Contact), Stripline, Low Power </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-39030/dtl 39030ss20.pdf </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">130 kb </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-39030 </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-DTL-39030/21B w/Amendment 1 -- Dated 1/31/2023 </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dummy Loads, Electrical, Type XIV (Tab Contact), Stripline, Medium Power </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-39030/dtl 39030ss21.pdf </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">108 kb </t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-39030 </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-DTL-83503 (Rev C) -- Dated 3/6/2023 </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Connectors, Electrical, Flat Cable, and/or Printed Wiring Board, Nonenvironmental General Specification for (w/Amendment 2) </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-83503/dtl 83503.pdf </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">288 kb </t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Document</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Description</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>File size</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>More info</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EP Study MIL-DTL-32139/15 and /16 -- Dated 4/5/2023 </t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Connectors, Electrical, Rectangular, Nanominiature, Dual Row, Plug, Receptacle, Polarized Shell, Pin, Sockets Contacts, Vertical PCB Surface Mount Shell </t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/5935EPStudies/eps dtl32139.pdf </t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">388 kb </t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= 5935EPStudies </t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-DTL-17/224A w/Amendment 1 -- Dated 2/27/2023 </t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cable, Radio Frequency, Flexible, Coaxial, 50 Ohms, Low Smoke, Low Loss Diameter .500 </t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-17/dtl17s s224.pdf </t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">117 kb </t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-17 </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-DTL-39030/20D w/Amendment 1 -- Dated 1/31/2023 </t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dummy Loads, Electrical Type XIV (Tab Contact), Stripline, Low Power </t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-39030/dtl 39030ss20.pdf </t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">130 kb </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-39030 </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-DTL-39030/21B w/Amendment 1 -- Dated 1/31/2023 </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dummy Loads, Electrical, Type XIV (Tab Contact), Stripline, Medium Power </t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-39030/dtl 39030ss21.pdf </t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">108 kb </t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Programs/MilSpec/ListDocs.aspx?BasicDoc= MIL-DTL-39030 </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MIL-DTL-83503 (Rev C) -- Dated 3/6/2023 </t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Connectors, Electrical, Flat Cable, and/or Printed Wiring Board, Nonenvironmental General Specification for (w/Amendment 2) </t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">https://landandmaritimeapps.dla.mil/Downloads/MilSpec/Docs/MIL-DTL-83503/dtl 83503.pdf </t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">288 kb </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>